<commit_message>
removed matched data from excel report
</commit_message>
<xml_diff>
--- a/src/main/resources/data1/Book1.xlsx
+++ b/src/main/resources/data1/Book1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manju\IdeaProjects\FileComparision\src\main\resources\data1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manju\IdeaProjects\filecomparision\src\main\resources\data1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D995CF9-2588-4C54-88C7-AD755C0AF737}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2471BB2F-2433-4BBE-842F-552AA51F9DCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0184327C-E070-46EE-AF30-BEB50419C72F}"/>
+    <workbookView xWindow="5088" yWindow="2604" windowWidth="17280" windowHeight="8880" xr2:uid="{0184327C-E070-46EE-AF30-BEB50419C72F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,13 +39,13 @@
     <t>TradeID</t>
   </si>
   <si>
-    <t>S</t>
+    <t>Risk</t>
   </si>
   <si>
-    <t>a</t>
+    <t>Curve</t>
   </si>
   <si>
-    <t>d</t>
+    <t>Type</t>
   </si>
 </sst>
 </file>
@@ -400,7 +400,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -424,7 +424,7 @@
         <v>1234</v>
       </c>
       <c r="B2">
-        <v>673</v>
+        <v>637.4</v>
       </c>
       <c r="C2">
         <v>537</v>

</xml_diff>

<commit_message>
multiple primary keys are handled
</commit_message>
<xml_diff>
--- a/src/main/resources/data1/Book1.xlsx
+++ b/src/main/resources/data1/Book1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manju\IdeaProjects\FileComparision\src\main\resources\data1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manju\IdeaProjects\filecomparision\src\main\resources\data1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D995CF9-2588-4C54-88C7-AD755C0AF737}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81078667-51F6-44E1-B37C-18D74592167E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0184327C-E070-46EE-AF30-BEB50419C72F}"/>
   </bookViews>
@@ -39,13 +39,13 @@
     <t>TradeID</t>
   </si>
   <si>
-    <t>S</t>
+    <t>Risk</t>
   </si>
   <si>
-    <t>a</t>
+    <t>Curve</t>
   </si>
   <si>
-    <t>d</t>
+    <t>Type</t>
   </si>
 </sst>
 </file>
@@ -81,8 +81,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -397,15 +400,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12A47E38-027D-4CEE-B36F-FB9DAA0B48A4}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -419,12 +422,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1234</v>
       </c>
       <c r="B2">
-        <v>673</v>
+        <v>637.4</v>
       </c>
       <c r="C2">
         <v>537</v>
@@ -433,7 +436,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1235</v>
       </c>
@@ -447,7 +450,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1236</v>
       </c>
@@ -461,7 +464,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1237</v>
       </c>
@@ -474,6 +477,9 @@
       <c r="D5">
         <v>738</v>
       </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F8" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>